<commit_message>
add Walking question data
</commit_message>
<xml_diff>
--- a/R/Felix/q7cq11eData.xlsx
+++ b/R/Felix/q7cq11eData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Community-Visioning/R/Felix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CFE4B4-D6C9-6C46-A382-38614C28A984}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA81D8-C465-244B-806C-74BAE63C8A60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15760" xr2:uid="{9AE7E273-AC85-224E-9256-BEE2236B4976}"/>
   </bookViews>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F712AFB3-7DB9-E246-AE6E-AE8A769A2D55}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9:V24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>